<commit_message>
updated excel and readme.txt
</commit_message>
<xml_diff>
--- a/2021_2022_proj_auto_avaliacao.xlsx
+++ b/2021_2022_proj_auto_avaliacao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t xml:space="preserve">Redes de Computadores 2021/2022</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">testes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.20.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">todos</t>
   </si>
   <si>
     <t xml:space="preserve">Auto-aval</t>
@@ -604,7 +610,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -643,6 +649,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -785,11 +795,11 @@
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.42"/>
@@ -844,49 +854,53 @@
       <c r="D6" s="5"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="13" t="s">
-        <v>8</v>
+      <c r="B11" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="14"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="n">
         <f aca="false">B13+F13</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4" t="n">
         <f aca="false">C13+G13</f>
@@ -894,29 +908,29 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="8" t="n">
         <f aca="false">SUM(B14:B31)</f>
-        <v>9</v>
+        <v>10.25</v>
       </c>
       <c r="C13" s="4" t="n">
         <f aca="false">SUM(C14:C31)</f>
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F13" s="8" t="n">
         <f aca="false">SUM(F14:F31)</f>
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="G13" s="4" t="n">
         <f aca="false">SUM(G14:G31)</f>
@@ -924,19 +938,19 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10" t="n">
+      <c r="A14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="11" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="10" t="n">
+      <c r="E14" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="n">
@@ -944,19 +958,19 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="10" t="n">
+      <c r="A15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="10" t="n">
+      <c r="E15" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="G15" s="1" t="n">
@@ -964,19 +978,19 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="10" t="n">
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="10" t="n">
+      <c r="E16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="G16" s="1" t="n">
@@ -984,19 +998,19 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="10" t="n">
+      <c r="A17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="10" t="n">
+      <c r="E17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="G17" s="1" t="n">
@@ -1004,19 +1018,19 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="10" t="n">
+      <c r="A18" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="10" t="n">
+      <c r="E18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="n">
@@ -1024,19 +1038,19 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="10" t="n">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="10" t="n">
+      <c r="E19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="n">
@@ -1044,19 +1058,19 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="10" t="n">
+      <c r="A20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="11" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="10" t="n">
+      <c r="E20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="n">
@@ -1064,19 +1078,19 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="10" t="n">
+      <c r="A21" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="10" t="n">
+      <c r="E21" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="G21" s="1" t="n">
@@ -1084,26 +1098,26 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="10" t="n">
+      <c r="A22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="10"/>
+      <c r="E22" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="11"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="10" t="n">
+      <c r="A23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="C23" s="1" t="n">
@@ -1111,46 +1125,46 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="10"/>
+      <c r="A24" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="B25" s="19"/>
       <c r="E25" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="10" t="n">
+      <c r="A27" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="11" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="10" t="n">
+      <c r="E27" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="n">
@@ -1158,19 +1172,19 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="10" t="n">
+      <c r="A28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="11" t="n">
         <v>2</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="10" t="n">
+      <c r="E28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="n">
@@ -1178,349 +1192,353 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="10"/>
+      <c r="A29" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="11" t="n">
+        <v>1.25</v>
+      </c>
       <c r="C29" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="10"/>
+      <c r="E29" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="11" t="n">
+        <v>0.75</v>
+      </c>
       <c r="G29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="E30" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="10"/>
+      <c r="A30" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="E30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="11"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="s">
-        <v>45</v>
+      <c r="A32" s="21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
-        <v>46</v>
+      <c r="A35" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="24" t="s">
-        <v>48</v>
+      <c r="E36" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="26" t="s">
+      <c r="A37" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F37" s="10" t="s">
-        <v>50</v>
+      <c r="B37" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>50</v>
+      <c r="A38" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>50</v>
+      <c r="A39" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>50</v>
+      <c r="A40" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>50</v>
+      <c r="A41" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>50</v>
+      <c r="A42" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>50</v>
+      <c r="A43" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>50</v>
+      <c r="A44" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>50</v>
+      <c r="A45" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>50</v>
+      <c r="A46" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>50</v>
+      <c r="A47" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F48" s="10" t="s">
+      <c r="A48" s="26" t="s">
         <v>74</v>
       </c>
+      <c r="B48" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="G48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49" s="24" t="s">
+      <c r="A49" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F50" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F49" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="G50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>50</v>
+      <c r="A51" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>74</v>
+      <c r="A52" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="G52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>50</v>
+      <c r="A53" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>74</v>
+      <c r="E54" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="G54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>50</v>
+      <c r="E55" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="G55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E56" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>88</v>
+      <c r="E56" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -1577,32 +1595,32 @@
       <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.93"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="D2" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="F2" s="29" t="s">
         <v>93</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
@@ -1614,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,12 +1649,12 @@
         <v>0.25</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.5</v>
@@ -1648,12 +1666,12 @@
         <v>0.5</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0.75</v>
@@ -1662,12 +1680,12 @@
         <v>0.75</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1</v>
@@ -1678,7 +1696,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>1.25</v>
@@ -1686,7 +1704,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>1.5</v>
@@ -1694,7 +1712,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>1.75</v>

</xml_diff>